<commit_message>
Add No Lag Figures
</commit_message>
<xml_diff>
--- a/code/misc/NoLagFigures/TripleInteractionBySex.xlsx
+++ b/code/misc/NoLagFigures/TripleInteractionBySex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bz22\Desktop\ComparativeMortality\code\misc\NoLagFigures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC45A0D-9D41-46F4-A23E-9B8F2A2858FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C57B1B8-6A31-4A87-87A7-EEB5CE588AE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1881B21E-1D1C-4E85-99DF-F396210C29B0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{1881B21E-1D1C-4E85-99DF-F396210C29B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -1253,7 +1253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89BB8C4C-4B3F-4C7B-A832-4F88A5573416}">
   <dimension ref="A1:KB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="IZ1" workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
@@ -7296,8 +7296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F360B43-9547-4622-951B-A82286483956}">
   <dimension ref="A1:G288"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
+      <selection activeCell="B179" sqref="B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>